<commit_message>
Added EditPage , EditPageBusinessLayer , EditPageErrorMessage
Added clickOnEditPageLinkOnSetUpLink()

Added tc001-tc006 tc of toggle

Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/ToggleData.xlsx
+++ b/ToggleData.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="EntityorAccount" sheetId="5" r:id="rId1"/>
     <sheet name="Fund" sheetId="6" r:id="rId2"/>
     <sheet name="Deal" sheetId="11" r:id="rId3"/>
+    <sheet name="CustomSDG" sheetId="12" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>Variable_Name</t>
   </si>
@@ -86,6 +87,24 @@
   </si>
   <si>
     <t>Deal Received</t>
+  </si>
+  <si>
+    <t>SDG_Name</t>
+  </si>
+  <si>
+    <t>SDG_Tag</t>
+  </si>
+  <si>
+    <t>sObjectName</t>
+  </si>
+  <si>
+    <t>TOGGLESDG1</t>
+  </si>
+  <si>
+    <t>Custom SDG</t>
+  </si>
+  <si>
+    <t>navpeII__Pipeline__c</t>
   </si>
 </sst>
 </file>
@@ -124,7 +143,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -143,6 +162,12 @@
         <bgColor rgb="FFA9D18E"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -158,7 +183,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -174,6 +199,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink 2" xfId="1"/>
@@ -832,7 +858,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
@@ -872,4 +898,52 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added DealPageBusinessLayer,DealPage, DealPageErrorMessage File
Added tc010-tc011 for Toggle

Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/ToggleData.xlsx
+++ b/ToggleData.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="EntityorAccount" sheetId="5" r:id="rId1"/>
     <sheet name="Fund" sheetId="6" r:id="rId2"/>
     <sheet name="Deal" sheetId="11" r:id="rId3"/>
     <sheet name="CustomSDG" sheetId="12" r:id="rId4"/>
-    <sheet name="ToggleBtn" sheetId="13" r:id="rId5"/>
+    <sheet name="DealRequestTracker" sheetId="14" r:id="rId5"/>
+    <sheet name="ToggleBtn" sheetId="13" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
   <si>
     <t>Variable_Name</t>
   </si>
@@ -115,6 +116,42 @@
   </si>
   <si>
     <t>Toggle_Button</t>
+  </si>
+  <si>
+    <t>OPENQA1</t>
+  </si>
+  <si>
+    <t>CLOSEDQA1</t>
+  </si>
+  <si>
+    <t>Request_Tracker_ID</t>
+  </si>
+  <si>
+    <t>Request</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>RT</t>
+  </si>
+  <si>
+    <t>Date_Requested</t>
+  </si>
+  <si>
+    <t>Finance Related</t>
+  </si>
+  <si>
+    <t>12/22/2020</t>
+  </si>
+  <si>
+    <t>12/7/2020</t>
+  </si>
+  <si>
+    <t>IT Related</t>
   </si>
 </sst>
 </file>
@@ -193,7 +230,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -210,6 +247,7 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink 2" xfId="1"/>
@@ -869,7 +907,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -915,7 +953,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -960,9 +998,78 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added tc012-tc013 of toggle
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/ToggleData.xlsx
+++ b/ToggleData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="EntityorAccount" sheetId="5" r:id="rId1"/>
@@ -1000,7 +1000,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -1069,8 +1069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Created/Overloded following method clickOnTab , clickOnAlreadyCreatedItem , getRelatedTab  , toggleSDGButtons ,toggleButton , toggleButtonColumnNames
MarketingEventPage,MarketingEventPageBusinessLayer java class added

Combined TC001 & TC010 IN TO ONE

Updated Toggle Excel

Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/ToggleData.xlsx
+++ b/ToggleData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="EntityorAccount" sheetId="5" r:id="rId1"/>
@@ -17,7 +17,9 @@
     <sheet name="Deal" sheetId="11" r:id="rId3"/>
     <sheet name="CustomSDG" sheetId="12" r:id="rId4"/>
     <sheet name="DealRequestTracker" sheetId="14" r:id="rId5"/>
-    <sheet name="ToggleBtn" sheetId="13" r:id="rId6"/>
+    <sheet name="MarketingEvent" sheetId="13" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="15" r:id="rId7"/>
+    <sheet name="ToggleButtonCheck" sheetId="16" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="74">
   <si>
     <t>Variable_Name</t>
   </si>
@@ -109,15 +111,6 @@
     <t>navpeII__Pipeline__c</t>
   </si>
   <si>
-    <t>Active Deals with All Stages !@#$%^&amp;*() @#$%^&amp;*Deals:Custom SDG</t>
-  </si>
-  <si>
-    <t>TOGGLEBTN1</t>
-  </si>
-  <si>
-    <t>Toggle_Button</t>
-  </si>
-  <si>
     <t>OPENQA1</t>
   </si>
   <si>
@@ -152,13 +145,121 @@
   </si>
   <si>
     <t>IT Related</t>
+  </si>
+  <si>
+    <t>Third Party Event</t>
+  </si>
+  <si>
+    <t>Alexa Event 1</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Organizer</t>
+  </si>
+  <si>
+    <t>2/10/2020</t>
+  </si>
+  <si>
+    <t>TOGGLEME1</t>
+  </si>
+  <si>
+    <t>Marketing_Event_Name</t>
+  </si>
+  <si>
+    <t>TabNAME&lt;BREAK&gt;ITEM&lt;BREAK&gt;RELATEDTAB&lt;BREAK&gt;1,2&lt;BREAK&gt;</t>
+  </si>
+  <si>
+    <t>Onject</t>
+  </si>
+  <si>
+    <t>TabNAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thirtd party </t>
+  </si>
+  <si>
+    <t>a,b ,c d</t>
+  </si>
+  <si>
+    <t>TabName</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>RelatedTab</t>
+  </si>
+  <si>
+    <t>ToggleButton</t>
+  </si>
+  <si>
+    <t>Entities</t>
+  </si>
+  <si>
+    <t>Investment</t>
+  </si>
+  <si>
+    <t>Fund Investments,Co-Investments</t>
+  </si>
+  <si>
+    <t>TBC1</t>
+  </si>
+  <si>
+    <t>TBC2</t>
+  </si>
+  <si>
+    <t>TBC3</t>
+  </si>
+  <si>
+    <t>Deals</t>
+  </si>
+  <si>
+    <t>Open Questions,Closed</t>
+  </si>
+  <si>
+    <t>Marketing Events</t>
+  </si>
+  <si>
+    <t>Overview</t>
+  </si>
+  <si>
+    <t>Third Party Event,Our Events</t>
+  </si>
+  <si>
+    <t>Q&amp;A</t>
+  </si>
+  <si>
+    <t>Column_Name1</t>
+  </si>
+  <si>
+    <t>Column_Name2</t>
+  </si>
+  <si>
+    <t>Legal Entity,Fund,Commitment Amount(M),Commitment Date</t>
+  </si>
+  <si>
+    <t>Legal Entity,Assest,Commitment Amount(M),Commitment Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Request Tracker ID,Date Requested,Request,Status,Response                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Request Tracker ID,Date Requested,Request,Response                                    </t>
+  </si>
+  <si>
+    <t>Name,Title,Email</t>
+  </si>
+  <si>
+    <t>Staff Name,Title,Mobile Phone</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -188,6 +289,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="5">
@@ -230,7 +337,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -248,6 +355,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink 2" xfId="1"/>
@@ -753,7 +861,7 @@
   <dimension ref="A1:ALP18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,7 +887,7 @@
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -907,7 +1015,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1016,47 +1124,47 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>38</v>
-      </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1067,32 +1175,221 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="64" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C3" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="108.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="57.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Test script related Verify the retain and default selection of Toggle button for each object for Toggle project
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/ToggleData.xlsx
+++ b/ToggleData.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="70">
   <si>
     <t>Variable_Name</t>
   </si>
@@ -201,9 +201,6 @@
     <t>Investment</t>
   </si>
   <si>
-    <t>Fund Investments,Co-Investments</t>
-  </si>
-  <si>
     <t>TBC1</t>
   </si>
   <si>
@@ -216,43 +213,34 @@
     <t>Deals</t>
   </si>
   <si>
-    <t>Open Questions,Closed</t>
-  </si>
-  <si>
     <t>Marketing Events</t>
   </si>
   <si>
     <t>Overview</t>
   </si>
   <si>
-    <t>Third Party Event,Our Events</t>
-  </si>
-  <si>
     <t>Q&amp;A</t>
   </si>
   <si>
-    <t>Column_Name1</t>
-  </si>
-  <si>
-    <t>Column_Name2</t>
-  </si>
-  <si>
-    <t>Legal Entity,Fund,Commitment Amount(M),Commitment Date</t>
-  </si>
-  <si>
-    <t>Legal Entity,Assest,Commitment Amount(M),Commitment Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Request Tracker ID,Date Requested,Request,Status,Response                             </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Request Tracker ID,Date Requested,Request,Response                                    </t>
-  </si>
-  <si>
-    <t>Name,Title,Email</t>
-  </si>
-  <si>
-    <t>Staff Name,Title,Mobile Phone</t>
+    <t>Column_Name</t>
+  </si>
+  <si>
+    <t>Fund Investments&lt;break&gt;Co-Investments</t>
+  </si>
+  <si>
+    <t>Open Questions&lt;break&gt;Closed</t>
+  </si>
+  <si>
+    <t>Third Party Event&lt;break&gt;Our Events</t>
+  </si>
+  <si>
+    <t>Legal Entity&lt;column&gt;Fund&lt;column&gt;Commitment Amount(M)&lt;column&gt;Commitment Date&lt;break&gt;Legal Entity&lt;column&gt;Asset&lt;column&gt;Commitment Amount(M)&lt;column&gt;Commitment Date</t>
+  </si>
+  <si>
+    <t>Request Tracker ID&lt;column&gt;Date Requested&lt;column&gt;Request&lt;column&gt;Status&lt;break&gt;Request Tracker ID&lt;column&gt;Date Requested&lt;column&gt;Request</t>
+  </si>
+  <si>
+    <t>Name&lt;column&gt;Title&lt;column&gt;Email&lt;break&gt;Staff Name&lt;column&gt;Title&lt;column&gt;Mobile Phone</t>
   </si>
 </sst>
 </file>
@@ -930,7 +918,7 @@
   <dimension ref="A1:AMK11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,7 +1003,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1109,7 +1097,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B2" sqref="B2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1284,10 +1272,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1297,10 +1285,10 @@
     <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.140625" customWidth="1"/>
     <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="57.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="127.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1317,15 +1305,12 @@
         <v>53</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
         <v>54</v>
@@ -1337,59 +1322,50 @@
         <v>55</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="F2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
       </c>
       <c r="D3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" t="s">
         <v>65</v>
       </c>
-      <c r="E3" t="s">
-        <v>61</v>
-      </c>
       <c r="F3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
         <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>